<commit_message>
Proceso de creación Explode Columns
</commit_message>
<xml_diff>
--- a/data/validation_excel/Malla_Emprendimiento_Colectivo.xlsx
+++ b/data/validation_excel/Malla_Emprendimiento_Colectivo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e94e71dc1438ec8/Escritorio/DIP/03_Malla_Validación/data/validation_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1269" documentId="8_{D967BF65-84EF-449F-8399-C69158E995BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40B9EA46-7325-4F35-989F-091434490D49}"/>
+  <xr:revisionPtr revIDLastSave="1298" documentId="8_{D967BF65-84EF-449F-8399-C69158E995BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D735D94B-CF5A-42A5-8096-575EC013AA5C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{406B4B18-D335-4FA1-B475-8E637F1B1B9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{406B4B18-D335-4FA1-B475-8E637F1B1B9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Validaciones" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Validaciones!$A$1:$F$244</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Valores!$A$1:$C$181</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Valores!$A$1:$C$182</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="313">
   <si>
     <t>Variable</t>
   </si>
@@ -965,6 +965,21 @@
   </si>
   <si>
     <t>list</t>
+  </si>
+  <si>
+    <t>En su vivienda|En un local o lote de su vivienda|En un local, vivienda, finca o terreno propio, diferente a su vivienda de habitación|En un local, vivienda, finca o terreno en arriendo o en aparcería|En una finca o un terreno ajeno con permiso del propietario (usufructo)|En una finca o un terreno ajeno sin permiso del propietario|En la calle como ambulante o como estacionario|En un quiosco o caseta|Puerta a puerta|En un vehículo (moto, taxi, carro, bus, lancha, barco, zorra o carreta)|En un territorio colectivo</t>
+  </si>
+  <si>
+    <t>Energía eléctrica|Alcantarillado|Gas natural|Recolección de basuras|Acueducto|Telefonía o Internet</t>
+  </si>
+  <si>
+    <t>Kilos|Toneladas|Litros|Unidades|Cabezas</t>
+  </si>
+  <si>
+    <t>La vereda - Corregimiento|Municipio|Departamento|Mercado Nacional|Mercado Internacional|Autoconsumo</t>
+  </si>
+  <si>
+    <t>1|2|3|4|5|6|7</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1077,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -1074,7 +1089,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30"/>
@@ -1400,8 +1416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4A26C9-6AFD-482D-88F5-D0E50D2070E1}">
   <dimension ref="A1:H244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B152" workbookViewId="0">
-      <selection activeCell="C162" sqref="C162"/>
+    <sheetView topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5264,10 +5280,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F3F87D-5E36-49F4-BD14-E381236E6911}">
-  <dimension ref="A1:C181"/>
+  <dimension ref="A1:C182"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6071,21 +6087,21 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>143</v>
+        <v>312</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>21</v>
+        <v>307</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>21</v>
@@ -6093,10 +6109,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>21</v>
@@ -6104,10 +6120,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>21</v>
@@ -6115,10 +6131,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>270</v>
+        <v>106</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>77</v>
+        <v>123</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>21</v>
@@ -6126,7 +6142,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>77</v>
@@ -6137,7 +6153,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>77</v>
@@ -6148,7 +6164,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>77</v>
@@ -6159,7 +6175,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>77</v>
@@ -6170,7 +6186,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>77</v>
@@ -6181,7 +6197,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>77</v>
@@ -6192,7 +6208,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>77</v>
@@ -6203,7 +6219,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>77</v>
@@ -6214,7 +6230,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>77</v>
@@ -6225,7 +6241,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>77</v>
@@ -6236,7 +6252,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>77</v>
@@ -6247,7 +6263,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>77</v>
@@ -6258,7 +6274,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>77</v>
@@ -6269,18 +6285,18 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>107</v>
+        <v>283</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>117</v>
+        <v>21</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>115</v>
@@ -6291,7 +6307,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>115</v>
@@ -6302,7 +6318,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>115</v>
@@ -6313,7 +6329,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>115</v>
@@ -6324,7 +6340,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>115</v>
@@ -6335,7 +6351,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>115</v>
@@ -6346,7 +6362,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>115</v>
@@ -6356,156 +6372,164 @@
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="2" t="s">
+      <c r="A99" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>304</v>
-      </c>
       <c r="C100" s="2" t="s">
-        <v>307</v>
+        <v>117</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
+        <v>161</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="7" t="s">
-        <v>305</v>
+        <v>163</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="7" t="s">
-        <v>164</v>
+        <v>305</v>
       </c>
       <c r="B103" s="2"/>
-      <c r="C103" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="C103" s="2"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B104" s="2"/>
-      <c r="C104" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="C104" s="2"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>249</v>
+        <v>310</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>117</v>
+        <v>307</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>117</v>
+        <v>307</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="C107" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>252</v>
-      </c>
       <c r="C108" s="2" t="s">
-        <v>117</v>
+        <v>307</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C109" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" s="7" t="s">
+      <c r="C110" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" s="2" t="s">
+      <c r="B111" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C111" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" s="7" t="s">
+      <c r="C112" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B112" s="2"/>
-      <c r="C112" s="11"/>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="B113" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>117</v>
+        <v>309</v>
+      </c>
+      <c r="C113" s="11" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>255</v>
+        <v>115</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>117</v>
@@ -6513,10 +6537,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>117</v>
@@ -6524,10 +6548,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>255</v>
+        <v>115</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>117</v>
@@ -6535,10 +6559,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>117</v>
@@ -6546,10 +6570,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>255</v>
+        <v>115</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>117</v>
@@ -6557,10 +6581,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>117</v>
@@ -6568,10 +6592,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>255</v>
+        <v>115</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>117</v>
@@ -6579,10 +6603,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>117</v>
@@ -6590,10 +6614,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>255</v>
+        <v>115</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>117</v>
@@ -6601,10 +6625,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>117</v>
@@ -6612,10 +6636,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>255</v>
+        <v>115</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>117</v>
@@ -6623,10 +6647,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>117</v>
@@ -6634,10 +6658,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>255</v>
+        <v>115</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>117</v>
@@ -6645,38 +6669,40 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B128" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C127" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128" s="7" t="s">
+      <c r="C128" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B128" s="2"/>
-      <c r="C128" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="B129" s="2" t="s">
-        <v>115</v>
+        <v>311</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>117</v>
+        <v>307</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>115</v>
@@ -6687,7 +6713,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>115</v>
@@ -6698,7 +6724,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>115</v>
@@ -6709,7 +6735,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>115</v>
@@ -6720,7 +6746,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>115</v>
@@ -6731,7 +6757,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>115</v>
@@ -6742,7 +6768,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>115</v>
@@ -6753,7 +6779,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>115</v>
@@ -6764,7 +6790,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>115</v>
@@ -6775,7 +6801,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>115</v>
@@ -6786,7 +6812,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>115</v>
@@ -6797,10 +6823,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>257</v>
+        <v>115</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>117</v>
@@ -6808,10 +6834,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>115</v>
+        <v>257</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>117</v>
@@ -6819,7 +6845,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>115</v>
@@ -6830,10 +6856,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>258</v>
+        <v>115</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>117</v>
@@ -6841,10 +6867,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>117</v>
@@ -6852,10 +6878,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>115</v>
+        <v>259</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>117</v>
@@ -6863,7 +6889,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>115</v>
@@ -6874,7 +6900,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>115</v>
@@ -6885,7 +6911,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>115</v>
@@ -6896,7 +6922,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>115</v>
@@ -6907,7 +6933,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>115</v>
@@ -6918,7 +6944,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>115</v>
@@ -6929,7 +6955,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>115</v>
@@ -6940,7 +6966,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>115</v>
@@ -6951,7 +6977,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>115</v>
@@ -6962,7 +6988,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>115</v>
@@ -6973,7 +6999,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B157" s="2" t="s">
         <v>115</v>
@@ -6984,7 +7010,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B158" s="2" t="s">
         <v>115</v>
@@ -6995,7 +7021,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B159" s="2" t="s">
         <v>115</v>
@@ -7006,10 +7032,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>260</v>
+        <v>115</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>117</v>
@@ -7017,47 +7043,43 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="B162" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C161" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A162" s="7" t="s">
+      <c r="C162" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A163" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="B162" s="2"/>
-      <c r="C162" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A163" s="7" t="s">
+      <c r="B163" s="2"/>
+      <c r="C163" s="2"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="B163" s="2"/>
-      <c r="C163" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A164" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="B164" s="2"/>
+      <c r="C164" s="2"/>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B165" s="3" t="s">
         <v>115</v>
@@ -7068,32 +7090,32 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A167" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B166" s="3" t="s">
+      <c r="B167" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="C166" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A167" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="B167" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C167" s="4" t="s">
+      <c r="C167" s="3" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>262</v>
+        <v>115</v>
       </c>
       <c r="C168" s="4" t="s">
         <v>117</v>
@@ -7101,10 +7123,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C169" s="4" t="s">
         <v>117</v>
@@ -7112,7 +7134,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B170" s="4" t="s">
         <v>263</v>
@@ -7123,7 +7145,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B171" s="4" t="s">
         <v>263</v>
@@ -7134,7 +7156,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B172" s="4" t="s">
         <v>263</v>
@@ -7145,7 +7167,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B173" s="4" t="s">
         <v>263</v>
@@ -7156,7 +7178,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B174" s="4" t="s">
         <v>263</v>
@@ -7166,19 +7188,19 @@
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A175" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="B175" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="C175" s="5" t="s">
+      <c r="A175" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="C175" s="4" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B176" s="5" t="s">
         <v>264</v>
@@ -7189,7 +7211,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B177" s="5" t="s">
         <v>264</v>
@@ -7200,10 +7222,10 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>115</v>
+        <v>264</v>
       </c>
       <c r="C178" s="5" t="s">
         <v>117</v>
@@ -7211,7 +7233,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B179" s="5" t="s">
         <v>115</v>
@@ -7222,7 +7244,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B180" s="5" t="s">
         <v>115</v>
@@ -7233,7 +7255,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B181" s="5" t="s">
         <v>115</v>
@@ -7242,8 +7264,19 @@
         <v>117</v>
       </c>
     </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A182" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B182" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C182" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C181" xr:uid="{51F3F87D-5E36-49F4-BD14-E381236E6911}"/>
+  <autoFilter ref="A1:C182" xr:uid="{51F3F87D-5E36-49F4-BD14-E381236E6911}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrección y Validación Malla
</commit_message>
<xml_diff>
--- a/data/validation_excel/Malla_Emprendimiento_Colectivo.xlsx
+++ b/data/validation_excel/Malla_Emprendimiento_Colectivo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e94e71dc1438ec8/Escritorio/DIP/03_Malla_Validación/data/validation_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1310" documentId="8_{D967BF65-84EF-449F-8399-C69158E995BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BC4D0B1-0EA3-4154-B266-3742349183C5}"/>
+  <xr:revisionPtr revIDLastSave="1314" documentId="8_{D967BF65-84EF-449F-8399-C69158E995BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EDF138F-17C8-42A7-A1D5-9056697FEC56}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{406B4B18-D335-4FA1-B475-8E637F1B1B9F}"/>
   </bookViews>
@@ -1419,8 +1419,8 @@
   <dimension ref="A1:H244"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F164" sqref="F164"/>
+      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B228" sqref="B228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5031,7 +5031,7 @@
         <v>228</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C227" s="3" t="s">
         <v>9</v>

</xml_diff>